<commit_message>
[WIP] fix boardcast status machine
</commit_message>
<xml_diff>
--- a/CIM.API/ProductionPlan/Pack plan 14 Jun 2020(for import).xlsx
+++ b/CIM.API/ProductionPlan/Pack plan 14 Jun 2020(for import).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\PSEC\Dole\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nprss\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F533A75-4AEE-46AC-BDEA-6D7B76EF6BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BF9EEF-5BE9-4F4A-944C-576E173936EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="14 Jun 20" sheetId="288" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'14 Jun 20'!$A$1:$S$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'14 Jun 20'!$A$1:$R$24</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +26,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="91">
   <si>
     <t xml:space="preserve"> QA: ______________________</t>
   </si>
@@ -138,9 +135,6 @@
   </si>
   <si>
     <t>หมายเหตุ</t>
-  </si>
-  <si>
-    <t>จำนวนเคส</t>
   </si>
   <si>
     <t>จำนวนไลน์</t>
@@ -233,12 +227,6 @@
     <t>ใช้มะม่วงพันธุ์ kaew item 500 เท่านั้น</t>
   </si>
   <si>
-    <t>Operating time</t>
-  </si>
-  <si>
-    <t>08.00-08.00</t>
-  </si>
-  <si>
     <t>Item Brite</t>
   </si>
   <si>
@@ -296,9 +284,6 @@
     <t>0.15 -0.60</t>
   </si>
   <si>
-    <t>20.00-08.00</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -311,16 +296,19 @@
     <t>date finish</t>
   </si>
   <si>
-    <t>13/06/2020 08:00</t>
-  </si>
-  <si>
     <t>เริ่มต้นอ่าน row ที่ 5 เป็นต้นไป</t>
   </si>
   <si>
     <t>ไม่อ่าน 2 row สุดท้าย</t>
   </si>
   <si>
-    <t>14/6/2020  14:00</t>
+    <t>13/06/2020 08:00 AM</t>
+  </si>
+  <si>
+    <t>14/6/2020  08:00 AM</t>
+  </si>
+  <si>
+    <t>จำนวน</t>
   </si>
 </sst>
 </file>
@@ -718,6 +706,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,6 +742,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -746,37 +755,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Currency 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal_Sheet1 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="สกุลเงิน" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1063,65 +1051,63 @@
     <tabColor theme="0" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="30" zoomScalePageLayoutView="10" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="30" zoomScalePageLayoutView="10" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="25.8"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="25.5"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="54" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="67.88671875" style="18" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" style="1" customWidth="1"/>
-    <col min="9" max="11" width="12.33203125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="7.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="54" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="67.85546875" style="18" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="12.28515625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="7.85546875" style="1" customWidth="1"/>
     <col min="14" max="17" width="16" style="12" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="12" customWidth="1"/>
-    <col min="19" max="19" width="34" style="1" customWidth="1"/>
-    <col min="20" max="20" width="17.33203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="20.109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="12" style="1"/>
+    <col min="18" max="18" width="34" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="12" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="33" customHeight="1">
-      <c r="A1" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-    </row>
-    <row r="2" spans="1:19" ht="26.4">
+    <row r="1" spans="1:18" ht="33" customHeight="1">
+      <c r="A1" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+    </row>
+    <row r="2" spans="1:18" ht="26.25">
       <c r="A2" s="42" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="50"/>
       <c r="D2" s="3"/>
       <c r="E2" s="42"/>
-      <c r="F2" s="71" t="s">
-        <v>91</v>
+      <c r="F2" s="57" t="s">
+        <v>86</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
@@ -1134,72 +1120,68 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:19" ht="21" customHeight="1">
-      <c r="A3" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="58" t="s">
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="1:18" ht="21" customHeight="1">
+      <c r="A3" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="58" t="s">
+      <c r="B3" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="C3" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="F3" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="G3" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="61" t="s">
+      <c r="H3" s="70" t="s">
         <v>37</v>
       </c>
+      <c r="I3" s="71"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="66" t="s">
+        <v>36</v>
+      </c>
       <c r="L3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="M3" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="P3" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q3" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="R3" s="56" t="s">
-        <v>64</v>
-      </c>
-      <c r="S3" s="58" t="s">
+      <c r="N3" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="P3" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q3" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" s="63" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="21" customHeight="1">
-      <c r="A4" s="62"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
+    <row r="4" spans="1:18" ht="21" customHeight="1">
+      <c r="A4" s="67"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="20" t="s">
         <v>32</v>
       </c>
@@ -1209,19 +1191,18 @@
       <c r="J4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="62"/>
+      <c r="K4" s="67"/>
       <c r="L4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="59"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="59"/>
-    </row>
-    <row r="5" spans="1:19" ht="59.4">
+      <c r="M4" s="64"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="64"/>
+    </row>
+    <row r="5" spans="1:18" ht="60.75">
       <c r="A5" s="32" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1210,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" s="43">
         <v>9334201</v>
@@ -1238,13 +1219,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="H5" s="48" t="s">
         <v>61</v>
-      </c>
-      <c r="H5" s="48" t="s">
-        <v>62</v>
       </c>
       <c r="I5" s="49" t="s">
         <v>12</v>
@@ -1253,7 +1234,7 @@
         <v>22</v>
       </c>
       <c r="K5" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L5" s="47" t="s">
         <v>27</v>
@@ -1265,52 +1246,49 @@
         <v>5000</v>
       </c>
       <c r="O5" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="P5" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="P5" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q5" s="70" t="s">
-        <v>93</v>
+      <c r="Q5" s="56" t="s">
+        <v>89</v>
       </c>
       <c r="R5" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S5" s="43" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="51.6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="60.75">
       <c r="A6" s="32"/>
       <c r="B6" s="44">
         <v>3</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D6" s="43">
         <v>93032018</v>
       </c>
       <c r="E6" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>52</v>
-      </c>
       <c r="G6" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H6" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="49" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K6" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L6" s="47" t="s">
         <v>27</v>
@@ -1321,15 +1299,14 @@
       <c r="N6" s="43"/>
       <c r="O6" s="43"/>
       <c r="P6" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q6" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R6" s="43"/>
-      <c r="S6" s="31"/>
-    </row>
-    <row r="7" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q6" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6" s="31"/>
+    </row>
+    <row r="7" spans="1:18" ht="60.75">
       <c r="A7" s="41" t="s">
         <v>26</v>
       </c>
@@ -1337,7 +1314,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" s="43">
         <v>93206101</v>
@@ -1372,25 +1349,22 @@
       <c r="N7" s="43"/>
       <c r="O7" s="43"/>
       <c r="P7" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q7" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R7" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S7" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q7" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R7" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="51">
       <c r="A8" s="41"/>
       <c r="B8" s="45">
         <v>8</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D8" s="43">
         <v>93440701</v>
@@ -1399,19 +1373,19 @@
         <v>9</v>
       </c>
       <c r="F8" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="35" t="s">
         <v>56</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>57</v>
       </c>
       <c r="H8" s="48" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="48" t="s">
         <v>58</v>
-      </c>
-      <c r="J8" s="48" t="s">
-        <v>59</v>
       </c>
       <c r="K8" s="48" t="s">
         <v>4</v>
@@ -1425,17 +1399,16 @@
       <c r="N8" s="43"/>
       <c r="O8" s="43"/>
       <c r="P8" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R8" s="43"/>
-      <c r="S8" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q8" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="51">
       <c r="A9" s="41" t="s">
         <v>25</v>
       </c>
@@ -1460,15 +1433,14 @@
       <c r="N9" s="43"/>
       <c r="O9" s="43"/>
       <c r="P9" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q9" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R9" s="43"/>
-      <c r="S9" s="34"/>
-    </row>
-    <row r="10" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R9" s="34"/>
+    </row>
+    <row r="10" spans="1:18" ht="51">
       <c r="A10" s="41" t="s">
         <v>24</v>
       </c>
@@ -1493,15 +1465,14 @@
       <c r="N10" s="43"/>
       <c r="O10" s="43"/>
       <c r="P10" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q10" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R10" s="43"/>
-      <c r="S10" s="34"/>
-    </row>
-    <row r="11" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q10" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10" s="34"/>
+    </row>
+    <row r="11" spans="1:18" ht="51">
       <c r="A11" s="41" t="s">
         <v>20</v>
       </c>
@@ -1515,22 +1486,22 @@
         <v>91720008</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H11" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="49" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J11" s="48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K11" s="48" t="s">
         <v>4</v>
@@ -1545,46 +1516,43 @@
         <v>7120</v>
       </c>
       <c r="O11" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="P11" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="P11" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q11" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R11" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S11" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="51.6">
+      <c r="Q11" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R11" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="51">
       <c r="A12" s="41"/>
       <c r="B12" s="45">
         <v>7</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D12" s="43">
         <v>9257108</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F12" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="49" t="s">
         <v>81</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="H12" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" s="49" t="s">
-        <v>84</v>
       </c>
       <c r="J12" s="48" t="s">
         <v>5</v>
@@ -1602,22 +1570,19 @@
         <v>2337</v>
       </c>
       <c r="O12" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="P12" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="P12" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q12" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R12" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S12" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="51.6">
+      <c r="Q12" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R12" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="51">
       <c r="A13" s="41" t="s">
         <v>19</v>
       </c>
@@ -1625,7 +1590,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="43">
         <v>93440701</v>
@@ -1634,19 +1599,19 @@
         <v>9</v>
       </c>
       <c r="F13" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="35" t="s">
         <v>56</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>57</v>
       </c>
       <c r="H13" s="48" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="48" t="s">
         <v>58</v>
-      </c>
-      <c r="J13" s="48" t="s">
-        <v>59</v>
       </c>
       <c r="K13" s="48" t="s">
         <v>4</v>
@@ -1660,19 +1625,16 @@
       <c r="N13" s="43"/>
       <c r="O13" s="43"/>
       <c r="P13" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q13" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R13" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="S13" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="64.8">
+        <v>88</v>
+      </c>
+      <c r="Q13" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R13" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="65.25">
       <c r="A14" s="41" t="s">
         <v>14</v>
       </c>
@@ -1680,7 +1642,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" s="43">
         <v>93297001</v>
@@ -1692,7 +1654,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="48" t="s">
         <v>7</v>
@@ -1715,19 +1677,16 @@
       <c r="N14" s="43"/>
       <c r="O14" s="43"/>
       <c r="P14" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q14" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R14" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S14" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" s="8" customFormat="1" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q14" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="8" customFormat="1" ht="51">
       <c r="A15" s="41" t="s">
         <v>13</v>
       </c>
@@ -1735,7 +1694,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D15" s="43">
         <v>93440701</v>
@@ -1744,19 +1703,19 @@
         <v>9</v>
       </c>
       <c r="F15" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>56</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>57</v>
       </c>
       <c r="H15" s="48" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="48" t="s">
         <v>58</v>
-      </c>
-      <c r="J15" s="48" t="s">
-        <v>59</v>
       </c>
       <c r="K15" s="48" t="s">
         <v>4</v>
@@ -1770,19 +1729,16 @@
       <c r="N15" s="43"/>
       <c r="O15" s="43"/>
       <c r="P15" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q15" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R15" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S15" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q15" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R15" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="60.75">
       <c r="A16" s="41" t="s">
         <v>11</v>
       </c>
@@ -1790,7 +1746,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D16" s="43">
         <v>93297001</v>
@@ -1802,7 +1758,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" s="48" t="s">
         <v>7</v>
@@ -1817,7 +1773,7 @@
         <v>4</v>
       </c>
       <c r="L16" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M16" s="48">
         <v>2</v>
@@ -1825,27 +1781,24 @@
       <c r="N16" s="43"/>
       <c r="O16" s="43"/>
       <c r="P16" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q16" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R16" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S16" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q16" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="60.75">
       <c r="A17" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="45">
         <v>8</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D17" s="43">
         <v>93206101</v>
@@ -1872,7 +1825,7 @@
         <v>4</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M17" s="48">
         <v>2</v>
@@ -1880,25 +1833,22 @@
       <c r="N17" s="43"/>
       <c r="O17" s="43"/>
       <c r="P17" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q17" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R17" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="S17" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="51.6">
+        <v>88</v>
+      </c>
+      <c r="Q17" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R17" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="51">
       <c r="A18" s="41"/>
       <c r="B18" s="45">
         <v>8</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D18" s="43">
         <v>93440701</v>
@@ -1907,25 +1857,25 @@
         <v>9</v>
       </c>
       <c r="F18" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="35" t="s">
         <v>56</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>57</v>
       </c>
       <c r="H18" s="48" t="s">
         <v>7</v>
       </c>
       <c r="I18" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="48" t="s">
         <v>58</v>
-      </c>
-      <c r="J18" s="48" t="s">
-        <v>59</v>
       </c>
       <c r="K18" s="48" t="s">
         <v>4</v>
       </c>
       <c r="L18" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M18" s="48">
         <v>2</v>
@@ -1933,17 +1883,16 @@
       <c r="N18" s="43"/>
       <c r="O18" s="43"/>
       <c r="P18" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q18" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="R18" s="43"/>
-      <c r="S18" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="36" customHeight="1">
+        <v>88</v>
+      </c>
+      <c r="Q18" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="R18" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="36" customHeight="1">
       <c r="A19" s="21" t="s">
         <v>3</v>
       </c>
@@ -1953,10 +1902,10 @@
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="I19" s="72"/>
+      <c r="H19" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="I19" s="60"/>
       <c r="J19" s="28"/>
       <c r="K19" s="27"/>
       <c r="L19" s="22"/>
@@ -1965,10 +1914,9 @@
       <c r="O19" s="22"/>
       <c r="P19" s="22"/>
       <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="29"/>
-    </row>
-    <row r="20" spans="1:19" ht="39.9" customHeight="1">
+      <c r="R19" s="29"/>
+    </row>
+    <row r="20" spans="1:18" ht="39.950000000000003" customHeight="1">
       <c r="A20" s="36" t="s">
         <v>2</v>
       </c>
@@ -1992,10 +1940,9 @@
       <c r="O20" s="37"/>
       <c r="P20" s="37"/>
       <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="7"/>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="R20" s="7"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="11"/>
       <c r="G21" s="13"/>
       <c r="H21" s="14"/>
@@ -2004,7 +1951,7 @@
       <c r="K21" s="16"/>
       <c r="L21" s="17"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:18">
       <c r="A22" s="11"/>
       <c r="G22" s="13"/>
       <c r="H22" s="14"/>
@@ -2014,14 +1961,9 @@
       <c r="L22" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
+  <mergeCells count="17">
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:R1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -2033,6 +1975,10 @@
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="R3:R4"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>